<commit_message>
updated with up board and case options
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markabrams/dev/kubecon-ai-demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECAB4B4-A717-D14B-B4E9-C1C0AEFB2DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ACA35F-79E3-B140-89F2-674D285AC3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{522825CF-1822-5348-A1ED-AA55215F150B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Jetson Xavier</t>
   </si>
@@ -73,12 +73,6 @@
     <t>Demo</t>
   </si>
   <si>
-    <t>Industrial Edge, Rancher, Fleet, K3s, Elemental</t>
-  </si>
-  <si>
-    <t>NUC</t>
-  </si>
-  <si>
     <t>Arduino</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>https://www.amazon.com/SAMSUNG-microSDXC-Expanded-MB-ME128KA-AM/dp/B09B1JFY24/ref=sr_1_3?keywords=128gb+micro+sd+card&amp;qid=1658949269&amp;sprefix=128%2Caps%2C82&amp;sr=8-3</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B09MZ2KW5G/ref=crt_ewc_title_oth_1?ie=UTF8&amp;smid=A3QBPG8WTLRGM2&amp;th=1</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/155</t>
   </si>
   <si>
@@ -185,6 +176,27 @@
   </si>
   <si>
     <t>Cooling Fan</t>
+  </si>
+  <si>
+    <t>Industrial Edge, Rancher, Fleet, K3s, Elemental (?)</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>UP4000</t>
+  </si>
+  <si>
+    <t>https://up-shop.org/up4000series.html</t>
+  </si>
+  <si>
+    <t>Travel case</t>
+  </si>
+  <si>
+    <t>https://nanuk.com/products/nanuk-935?variant=37067405983904</t>
+  </si>
+  <si>
+    <t>All demos listed</t>
   </si>
 </sst>
 </file>
@@ -244,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -257,6 +269,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE10576-FE4A-8045-8801-6435ADEBA4DF}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,376 +621,426 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="8">
+        <f>SUM(J11,J28)</f>
+        <v>935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6">
-        <f>F3*G3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="6">
-        <v>40</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
-        <f>F4*G4</f>
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F5" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" s="6">
         <f>F5*G5</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6">
         <v>40</v>
-      </c>
-      <c r="F6" s="6">
-        <v>30</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="6">
         <f>F6*G6</f>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>44</v>
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="6">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" s="6">
         <f>F7*G7</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="6">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <f>F8*G8</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1</v>
+      </c>
       <c r="H9" s="6">
-        <f>SUM(H3:H7)</f>
+        <f>F9*G9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11" s="6">
+        <f>SUM(H5:H9)</f>
         <v>95</v>
       </c>
-      <c r="I9">
+      <c r="I11">
         <v>2</v>
       </c>
-      <c r="J9" s="7">
-        <f>H9*I9</f>
+      <c r="J11" s="7">
+        <f>H11*I11</f>
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="6">
-        <v>650</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6">
-        <f>F12*G12</f>
-        <v>650</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="6">
-        <v>30</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="6">
-        <f t="shared" ref="H13:H22" si="0">F13*G13</f>
-        <v>30</v>
+    <row r="13" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
       </c>
       <c r="F14" s="6">
+        <v>260</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <f>F14*G14</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="6">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" ref="H15:H25" si="0">F15*G15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6">
         <v>12</v>
       </c>
-      <c r="G14">
+      <c r="G16">
         <v>6</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H16" s="6">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="6">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="6">
         <v>18</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="6">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="6">
-        <v>15</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="6">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="6">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6">
         <v>26</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="6">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6">
         <v>26</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="6">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="6">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="6">
         <v>30</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" s="6">
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="6">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="6">
         <v>5</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="6">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="6">
         <v>18</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21" s="6">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="6">
         <v>15</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D23" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="6">
+        <v>230</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H28" s="6">
+        <f>SUM(H14:H25)</f>
+        <v>745</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="7">
+        <f>H28*I28</f>
+        <v>745</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H25" s="6">
-        <f>SUM(H12:H22)</f>
-        <v>905</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25" s="7">
-        <f>H25*I25</f>
-        <v>905</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>38</v>
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{D4E798D5-1360-D249-ACD8-9C2008A7C5A9}"/>
-    <hyperlink ref="E14" r:id="rId2" xr:uid="{27BF099E-5D16-1E41-B6CF-AFCB7571CF4B}"/>
-    <hyperlink ref="E17" r:id="rId3" xr:uid="{1F2BDFE0-8CF6-034B-B9E9-CDFED5E8D89D}"/>
-    <hyperlink ref="E18" r:id="rId4" xr:uid="{61462C51-3FE1-B442-B88E-EFD6474BB46E}"/>
-    <hyperlink ref="E20" r:id="rId5" xr:uid="{EC18D8EA-94AC-1842-AF72-94FBDBE0F25F}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{D4E798D5-1360-D249-ACD8-9C2008A7C5A9}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{27BF099E-5D16-1E41-B6CF-AFCB7571CF4B}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{1F2BDFE0-8CF6-034B-B9E9-CDFED5E8D89D}"/>
+    <hyperlink ref="E20" r:id="rId4" xr:uid="{61462C51-3FE1-B442-B88E-EFD6474BB46E}"/>
+    <hyperlink ref="E22" r:id="rId5" xr:uid="{EC18D8EA-94AC-1842-AF72-94FBDBE0F25F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>